<commit_message>
[UPDATE] se actualiza query de modelo-ER.txt sin verificacion de funcionamiento
</commit_message>
<xml_diff>
--- a/disenno_modelo_entidad_relacional_tablas_entidades.xlsx
+++ b/disenno_modelo_entidad_relacional_tablas_entidades.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
     <sheet name="detalle_pedido" sheetId="10" r:id="rId10"/>
     <sheet name="estado_pedido" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,6 +48,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
+    <t>ENTIDAD POSTERS</t>
+  </si>
+  <si>
     <t>poster_id</t>
   </si>
   <si>
@@ -63,16 +66,19 @@
     <t>poster_stock</t>
   </si>
   <si>
-    <t>ENTIDAD POSTERS</t>
-  </si>
-  <si>
     <t>tamanno_id</t>
   </si>
   <si>
+    <t>catagoria_id</t>
+  </si>
+  <si>
+    <t>Entidad tamanno descripcion</t>
+  </si>
+  <si>
     <t>tamanno_descripcion</t>
   </si>
   <si>
-    <t>Entidad tamanno descripcion</t>
+    <t>Entidad usuarios</t>
   </si>
   <si>
     <t>usuario_id</t>
@@ -93,7 +99,7 @@
     <t>usuario_contrasenna</t>
   </si>
   <si>
-    <t>Entidad usuarios</t>
+    <t>Entidad roles</t>
   </si>
   <si>
     <t>rol_id</t>
@@ -102,19 +108,19 @@
     <t>rol_nombre</t>
   </si>
   <si>
-    <t>Entidad roles</t>
-  </si>
-  <si>
     <t>Entidad usuarios roles</t>
   </si>
   <si>
+    <t>Entidad categoria</t>
+  </si>
+  <si>
     <t>categoria_id</t>
   </si>
   <si>
     <t>categoria_nombre</t>
   </si>
   <si>
-    <t>Entidad categoria</t>
+    <t>Entidad de carrito compras</t>
   </si>
   <si>
     <t>carrito_compra_id</t>
@@ -123,7 +129,7 @@
     <t>fecha_creacion</t>
   </si>
   <si>
-    <t>Entidad de carrito compras</t>
+    <t>Entidad detalle carrito</t>
   </si>
   <si>
     <t>detalle_carrito_id</t>
@@ -132,23 +138,17 @@
     <t>detalle_carrito_cantidad</t>
   </si>
   <si>
-    <t>Entidad detalle carrito</t>
-  </si>
-  <si>
     <t>pedido_id</t>
   </si>
   <si>
     <t>pedi</t>
-  </si>
-  <si>
-    <t>catagoria_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -227,9 +227,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -250,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -552,47 +549,47 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8">
       <c r="B1" s="6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="2:8">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -603,7 +600,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -614,7 +611,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -625,7 +622,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -650,7 +647,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -664,7 +661,7 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -678,82 +675,82 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3">
       <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
@@ -773,18 +770,18 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7">
       <c r="B1" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -792,27 +789,27 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -820,7 +817,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -828,7 +825,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -836,7 +833,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -844,7 +841,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -852,7 +849,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -860,7 +857,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -868,7 +865,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -876,7 +873,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -884,7 +881,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -892,7 +889,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -900,7 +897,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -908,7 +905,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -916,7 +913,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -924,7 +921,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -932,7 +929,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -940,7 +937,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -948,7 +945,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -972,98 +969,98 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3">
       <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
@@ -1083,95 +1080,95 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3">
       <c r="B1" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
@@ -1191,99 +1188,99 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3">
       <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4" s="2"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3">
       <c r="B5" s="2"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3">
       <c r="B6" s="2"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3">
       <c r="B7" s="2"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3">
       <c r="B8" s="2"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9" s="2"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3">
       <c r="B10" s="2"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3">
       <c r="B11" s="2"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3">
       <c r="B12" s="2"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3">
       <c r="B13" s="2"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3">
       <c r="B14" s="2"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3">
       <c r="B15" s="2"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3">
       <c r="B16" s="2"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3">
       <c r="B17" s="2"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3">
       <c r="B18" s="2"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3">
       <c r="B19" s="2"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3">
       <c r="B20" s="2"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3">
       <c r="B21" s="2"/>
       <c r="C21" s="5"/>
     </row>
@@ -1303,91 +1300,91 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4">
       <c r="B1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1408,138 +1405,138 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5">
       <c r="B1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5">
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1561,17 +1558,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>